<commit_message>
RESULTS - stable version - project 22 mistake (r=0.3) corrected (setting to investigate) old result documented in project.py
</commit_message>
<xml_diff>
--- a/reports/~opt_report - final.xlsx
+++ b/reports/~opt_report - final.xlsx
@@ -8,19 +8,54 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iesegnet-my.sharepoint.com/personal/s_rostami_ieseg_fr/Documents/Research/Papers/2020-eNPV_Contract/NPV Risk Contract - Python/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{C3D5CD49-C27D-46BC-859D-A52C2A0BD00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C126DA2B-88B7-4AFF-9E7F-03AC8FB14796}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{C3D5CD49-C27D-46BC-859D-A52C2A0BD00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A59A47B1-FA3B-4CD1-BB2F-CEC99BD16935}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="38370" windowHeight="20850" xr2:uid="{A15588AD-266E-453F-8B7B-E3EF722B19C5}"/>
+    <workbookView xWindow="25490" yWindow="-3760" windowWidth="38620" windowHeight="21100" xr2:uid="{A15588AD-266E-453F-8B7B-E3EF722B19C5}"/>
   </bookViews>
   <sheets>
     <sheet name="~opt_report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="23">
   <si>
     <t xml:space="preserve">time      </t>
   </si>
@@ -82,7 +117,13 @@
     <t xml:space="preserve">tm        </t>
   </si>
   <si>
-    <t>dif</t>
+    <t>tvar</t>
+  </si>
+  <si>
+    <t>opt gap</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -566,9 +607,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -625,6 +670,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -944,10 +993,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{375C455C-17BC-47B1-9F08-29BAFD68187D}">
-  <dimension ref="A1:T105"/>
+  <dimension ref="A1:Z105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,9 +1015,16 @@
     <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" customWidth="1"/>
+    <col min="26" max="26" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1016,11 +1073,22 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45947.98541666667</v>
       </c>
@@ -1069,17 +1137,35 @@
       <c r="P2">
         <v>-23728.748870830001</v>
       </c>
-      <c r="R2">
-        <v>0.13</v>
-      </c>
-      <c r="S2">
-        <v>0.11</v>
-      </c>
-      <c r="T2">
-        <v>49.62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V2" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45947.98541666667</v>
       </c>
@@ -1128,8 +1214,42 @@
       <c r="P3">
         <v>-19581.01250298</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>22</v>
+      </c>
+      <c r="S3">
+        <v>50000</v>
+      </c>
+      <c r="T3" cm="1">
+        <f t="array" ref="T3">_xlfn._xlws.FILTER($P:$P,($B:$B=$R3)*($C:$C=T$2))</f>
+        <v>-13138.35738379</v>
+      </c>
+      <c r="U3" cm="1">
+        <f t="array" ref="U3">_xlfn._xlws.FILTER($P:$P,($B:$B=$R3)*($C:$C=U$2))</f>
+        <v>-11291.92386407</v>
+      </c>
+      <c r="V3" cm="1">
+        <f t="array" ref="V3">_xlfn._xlws.FILTER($P:$P,($B:$B=$R3)*($C:$C=V$2))</f>
+        <v>-13138.35738379</v>
+      </c>
+      <c r="W3" cm="1">
+        <f t="array" ref="W3">_xlfn._xlws.FILTER($P:$P,($B:$B=$R3)*($C:$C=W$2))</f>
+        <v>-11291.92386407</v>
+      </c>
+      <c r="X3">
+        <f>IF(100*ABS(T3-$W3)/ABS($W3)&gt;$R$1,100*ABS(T3-$W3)/ABS($W3),0)</f>
+        <v>16.351806317036939</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Z3" si="0">IF(100*ABS(U3-$W3)/ABS($W3)&gt;$R$1,100*ABS(U3-$W3)/ABS($W3),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" si="0"/>
+        <v>16.351806317036939</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45947.98541666667</v>
       </c>
@@ -1178,8 +1298,42 @@
       <c r="P4">
         <v>-23728.748870830001</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>23</v>
+      </c>
+      <c r="S4">
+        <v>75000</v>
+      </c>
+      <c r="T4" cm="1">
+        <f t="array" ref="T4">_xlfn._xlws.FILTER($P:$P,($B:$B=$R4)*($C:$C=T$2))</f>
+        <v>-18433.553127309999</v>
+      </c>
+      <c r="U4" cm="1">
+        <f t="array" ref="U4">_xlfn._xlws.FILTER($P:$P,($B:$B=$R4)*($C:$C=U$2))</f>
+        <v>-15121.20811654</v>
+      </c>
+      <c r="V4" cm="1">
+        <f t="array" ref="V4">_xlfn._xlws.FILTER($P:$P,($B:$B=$R4)*($C:$C=V$2))</f>
+        <v>-18433.553127309999</v>
+      </c>
+      <c r="W4" cm="1">
+        <f t="array" ref="W4">_xlfn._xlws.FILTER($P:$P,($B:$B=$R4)*($C:$C=W$2))</f>
+        <v>-15121.20811654</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ref="X4:X8" si="1">IF(100*ABS(T4-$W4)/ABS($W4)&gt;$R$1,100*ABS(T4-$W4)/ABS($W4),0)</f>
+        <v>21.905293447729644</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y8" si="2">IF(100*ABS(U4-$W4)/ABS($W4)&gt;$R$1,100*ABS(U4-$W4)/ABS($W4),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" ref="Z4:Z8" si="3">IF(100*ABS(V4-$W4)/ABS($W4)&gt;$R$1,100*ABS(V4-$W4)/ABS($W4),0)</f>
+        <v>21.905293447729644</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45947.98541666667</v>
       </c>
@@ -1228,8 +1382,42 @@
       <c r="P5">
         <v>-19581.01250298</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>100000</v>
+      </c>
+      <c r="T5" cm="1">
+        <f t="array" ref="T5">_xlfn._xlws.FILTER($P:$P,($B:$B=$R5)*($C:$C=T$2))</f>
+        <v>-23728.748870830001</v>
+      </c>
+      <c r="U5" cm="1">
+        <f t="array" ref="U5">_xlfn._xlws.FILTER($P:$P,($B:$B=$R5)*($C:$C=U$2))</f>
+        <v>-19581.01250298</v>
+      </c>
+      <c r="V5" cm="1">
+        <f t="array" ref="V5">_xlfn._xlws.FILTER($P:$P,($B:$B=$R5)*($C:$C=V$2))</f>
+        <v>-23728.748870830001</v>
+      </c>
+      <c r="W5" cm="1">
+        <f t="array" ref="W5">_xlfn._xlws.FILTER($P:$P,($B:$B=$R5)*($C:$C=W$2))</f>
+        <v>-19581.01250298</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="1"/>
+        <v>21.182440730369606</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="3"/>
+        <v>21.182440730369606</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45947.985925925925</v>
       </c>
@@ -1278,8 +1466,42 @@
       <c r="P6">
         <v>-25044.314767219999</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>24</v>
+      </c>
+      <c r="S6">
+        <v>150000</v>
+      </c>
+      <c r="T6" cm="1">
+        <f t="array" ref="T6">_xlfn._xlws.FILTER($P:$P,($B:$B=$R6)*($C:$C=T$2))</f>
+        <v>-34319.140357880002</v>
+      </c>
+      <c r="U6" cm="1">
+        <f t="array" ref="U6">_xlfn._xlws.FILTER($P:$P,($B:$B=$R6)*($C:$C=U$2))</f>
+        <v>-29130.252439669999</v>
+      </c>
+      <c r="V6" cm="1">
+        <f t="array" ref="V6">_xlfn._xlws.FILTER($P:$P,($B:$B=$R6)*($C:$C=V$2))</f>
+        <v>-34319.140357880002</v>
+      </c>
+      <c r="W6" cm="1">
+        <f t="array" ref="W6">_xlfn._xlws.FILTER($P:$P,($B:$B=$R6)*($C:$C=W$2))</f>
+        <v>-29130.252439669999</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="1"/>
+        <v>17.812711815513484</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="3"/>
+        <v>17.812711815513484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45947.985925925925</v>
       </c>
@@ -1328,8 +1550,42 @@
       <c r="P7">
         <v>-19581.01250298</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>25</v>
+      </c>
+      <c r="S7">
+        <v>200000</v>
+      </c>
+      <c r="T7" cm="1">
+        <f t="array" ref="T7">_xlfn._xlws.FILTER($P:$P,($B:$B=$R7)*($C:$C=T$2))</f>
+        <v>-44909.531844919999</v>
+      </c>
+      <c r="U7" cm="1">
+        <f t="array" ref="U7">_xlfn._xlws.FILTER($P:$P,($B:$B=$R7)*($C:$C=U$2))</f>
+        <v>-39078.902980610001</v>
+      </c>
+      <c r="V7" cm="1">
+        <f t="array" ref="V7">_xlfn._xlws.FILTER($P:$P,($B:$B=$R7)*($C:$C=V$2))</f>
+        <v>-44909.531844919999</v>
+      </c>
+      <c r="W7" cm="1">
+        <f t="array" ref="W7">_xlfn._xlws.FILTER($P:$P,($B:$B=$R7)*($C:$C=W$2))</f>
+        <v>-39078.902980610001</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="1"/>
+        <v>14.920144680629887</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="3"/>
+        <v>14.920144680629887</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45947.985925925925</v>
       </c>
@@ -1378,8 +1634,42 @@
       <c r="P8">
         <v>-25044.314767219999</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>26</v>
+      </c>
+      <c r="S8">
+        <v>250000</v>
+      </c>
+      <c r="T8" cm="1">
+        <f t="array" ref="T8">_xlfn._xlws.FILTER($P:$P,($B:$B=$R8)*($C:$C=T$2))</f>
+        <v>-55499.92333197</v>
+      </c>
+      <c r="U8" cm="1">
+        <f t="array" ref="U8">_xlfn._xlws.FILTER($P:$P,($B:$B=$R8)*($C:$C=U$2))</f>
+        <v>-49246.850205909999</v>
+      </c>
+      <c r="V8" cm="1">
+        <f t="array" ref="V8">_xlfn._xlws.FILTER($P:$P,($B:$B=$R8)*($C:$C=V$2))</f>
+        <v>-55499.92333197</v>
+      </c>
+      <c r="W8" cm="1">
+        <f t="array" ref="W8">_xlfn._xlws.FILTER($P:$P,($B:$B=$R8)*($C:$C=W$2))</f>
+        <v>-49246.850205909999</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="1"/>
+        <v>12.697407245163436</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="3"/>
+        <v>12.697407245163436</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45947.985925925925</v>
       </c>
@@ -1428,8 +1718,20 @@
       <c r="P9">
         <v>-19581.01250298</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X9" t="str" cm="1">
+        <f t="array" ref="X9">_xlfn.TEXTJOIN("", TRUE, "(" &amp; $S$3:$S$8 &amp; ", " &amp; X3:X8 &amp; ") ")</f>
+        <v xml:space="preserve">(50000, 16.3518063170369) (75000, 21.9052934477296) (100000, 21.1824407303696) (150000, 17.8127118155135) (200000, 14.9201446806299) (250000, 12.6974072451634) </v>
+      </c>
+      <c r="Y9" t="str" cm="1">
+        <f t="array" ref="Y9">_xlfn.TEXTJOIN("", TRUE, "(" &amp; $S$3:$S$8 &amp; ", " &amp; Y3:Y8 &amp; ") ")</f>
+        <v xml:space="preserve">(50000, 0) (75000, 0) (100000, 0) (150000, 0) (200000, 0) (250000, 0) </v>
+      </c>
+      <c r="Z9" t="str" cm="1">
+        <f t="array" ref="Z9">_xlfn.TEXTJOIN("", TRUE, "(" &amp; $S$3:$S$8 &amp; ", " &amp; Z3:Z8 &amp; ") ")</f>
+        <v xml:space="preserve">(50000, 16.3518063170369) (75000, 21.9052934477296) (100000, 21.1824407303696) (150000, 17.8127118155135) (200000, 14.9201446806299) (250000, 12.6974072451634) </v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45947.98642361111</v>
       </c>
@@ -1478,8 +1780,22 @@
       <c r="P10">
         <v>-24473.25574651</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X10" t="str">
+        <f>"\addplot+[mark=square*] coordinates {"
+        &amp;Z9&amp;
+      "};
+      \addlegendentry{lh}
+      \addplot+[mark=triangle*] coordinates {"
+        &amp;Y9&amp;
+      "};
+      \addlegendentry{cp}"</f>
+        <v>\addplot+[mark=square*] coordinates {(50000, 16.3518063170369) (75000, 21.9052934477296) (100000, 21.1824407303696) (150000, 17.8127118155135) (200000, 14.9201446806299) (250000, 12.6974072451634) };
+      \addlegendentry{lh}
+      \addplot+[mark=triangle*] coordinates {(50000, 0) (75000, 0) (100000, 0) (150000, 0) (200000, 0) (250000, 0) };
+      \addlegendentry{cp}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45947.98642361111</v>
       </c>
@@ -1529,7 +1845,7 @@
         <v>-19581.01250298</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45947.98642361111</v>
       </c>
@@ -1579,7 +1895,7 @@
         <v>-24473.25574651</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45947.98642361111</v>
       </c>
@@ -1629,7 +1945,7 @@
         <v>-19581.01250298</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45947.986921296295</v>
       </c>
@@ -1679,7 +1995,7 @@
         <v>-23003.34567617</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45947.986921296295</v>
       </c>
@@ -1729,7 +2045,7 @@
         <v>-19581.01250298</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45947.986921296295</v>
       </c>
@@ -5229,9 +5545,9 @@
         <v>-12678.939775770001</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>45947.996238425927</v>
+        <v>45948.663611111115</v>
       </c>
       <c r="B86">
         <v>22</v>
@@ -5240,7 +5556,7 @@
         <v>16</v>
       </c>
       <c r="D86">
-        <v>59572.044600000001</v>
+        <v>37261.088199999998</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -5252,36 +5568,27 @@
         <v>5000</v>
       </c>
       <c r="H86">
-        <v>-2449.8448173100001</v>
+        <v>7600.2892416699997</v>
       </c>
       <c r="I86">
-        <v>36.553699999999999</v>
+        <v>30.001638710000002</v>
       </c>
       <c r="J86">
-        <v>36.632511909999998</v>
-      </c>
-      <c r="K86">
-        <v>0</v>
-      </c>
-      <c r="L86">
         <v>0</v>
       </c>
       <c r="M86">
-        <v>-8126.3800859200001</v>
+        <v>-10440.156118250001</v>
       </c>
       <c r="N86">
-        <v>-3745.8014409699999</v>
-      </c>
-      <c r="O86">
-        <v>-11882.630120489999</v>
+        <v>-2698.20126553</v>
       </c>
       <c r="P86">
-        <v>-11872.181526890001</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-13138.35738379</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>45947.996238425927</v>
+        <v>45948.663611111115</v>
       </c>
       <c r="B87">
         <v>22</v>
@@ -5290,10 +5597,10 @@
         <v>17</v>
       </c>
       <c r="D87">
-        <v>57558.930899999999</v>
+        <v>26249.485799999999</v>
       </c>
       <c r="E87">
-        <v>7.8899999999999998E-2</v>
+        <v>0.43180000000000002</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -5302,36 +5609,27 @@
         <v>5000</v>
       </c>
       <c r="H87">
-        <v>-2449.8448173100001</v>
+        <v>7600.2892416699997</v>
       </c>
       <c r="I87">
-        <v>36.356499999999997</v>
+        <v>14.813225210000001</v>
       </c>
       <c r="J87">
-        <v>36.360640060000001</v>
-      </c>
-      <c r="K87">
-        <v>0.65290000000000004</v>
-      </c>
-      <c r="L87">
-        <v>0.64387119999999998</v>
+        <v>4.1046126200000002</v>
       </c>
       <c r="M87">
-        <v>-8067.2409788599998</v>
+        <v>-6415.7601938300004</v>
       </c>
       <c r="N87">
-        <v>-3730.6523803999999</v>
-      </c>
-      <c r="O87">
-        <v>-11804.69683506</v>
+        <v>-4876.1636702400001</v>
       </c>
       <c r="P87">
-        <v>-11797.893359260001</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-11291.92386407</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>45947.996238425927</v>
+        <v>45948.663611111115</v>
       </c>
       <c r="B88">
         <v>22</v>
@@ -5340,48 +5638,39 @@
         <v>18</v>
       </c>
       <c r="D88">
-        <v>38873.704400000002</v>
+        <v>37261.088199999998</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="F88">
-        <v>5617.0608000000002</v>
+        <v>0</v>
       </c>
       <c r="G88">
         <v>5000</v>
       </c>
       <c r="H88">
-        <v>-2449.8448173100001</v>
+        <v>7600.2892416699997</v>
       </c>
       <c r="I88">
-        <v>16.841999999999999</v>
+        <v>30.001638710000002</v>
       </c>
       <c r="J88">
-        <v>16.880077119999999</v>
-      </c>
-      <c r="K88">
-        <v>0</v>
-      </c>
-      <c r="L88">
         <v>0</v>
       </c>
       <c r="M88">
-        <v>-6153.0149303600001</v>
+        <v>-10440.156118250001</v>
       </c>
       <c r="N88">
-        <v>-1343.55495868</v>
-      </c>
-      <c r="O88">
-        <v>-7488.3837579499996</v>
+        <v>-2698.20126553</v>
       </c>
       <c r="P88">
-        <v>-7496.56988903</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-13138.35738379</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>45947.996238425927</v>
+        <v>45948.663611111115</v>
       </c>
       <c r="B89">
         <v>22</v>
@@ -5390,43 +5679,34 @@
         <v>19</v>
       </c>
       <c r="D89">
-        <v>38380.0262</v>
+        <v>23369.092199999999</v>
       </c>
       <c r="E89">
-        <v>1.0999999999999999E-2</v>
+        <v>0.5</v>
       </c>
       <c r="F89">
-        <v>5675.1854000000003</v>
+        <v>236.24539999999999</v>
       </c>
       <c r="G89">
         <v>5000</v>
       </c>
       <c r="H89">
-        <v>-2449.8448173100001</v>
+        <v>7600.2892416699997</v>
       </c>
       <c r="I89">
-        <v>16.6294</v>
+        <v>9.4715372700000007</v>
       </c>
       <c r="J89">
-        <v>16.59037528</v>
-      </c>
-      <c r="K89">
-        <v>0</v>
-      </c>
-      <c r="L89">
-        <v>0</v>
+        <v>9.9272690000000008</v>
       </c>
       <c r="M89">
-        <v>-6125.6850698899998</v>
+        <v>-5610.9562241599997</v>
       </c>
       <c r="N89">
-        <v>-1362.0270959899999</v>
-      </c>
-      <c r="O89">
-        <v>-7480.1725341600004</v>
+        <v>-5680.9676399199998</v>
       </c>
       <c r="P89">
-        <v>-7487.7121658799997</v>
+        <v>-11291.92386407</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -6230,6 +6510,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="X1:Z1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>